<commit_message>
updates years to include
</commit_message>
<xml_diff>
--- a/data-raw/metadata/clear_years_to_include_metadata.xlsx
+++ b/data-raw/metadata/clear_years_to_include_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-clear-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D55FEFC-D95E-374D-9814-69A04A7B985B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EBA2D8-81EF-5F4A-B6E9-2BD4C8549A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,9 +97,6 @@
     <t>2023</t>
   </si>
   <si>
-    <t>removed</t>
-  </si>
-  <si>
     <t>Indicates if year should be removed from analysis if TRUE</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t>brood_year</t>
+  </si>
+  <si>
+    <t>remove</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -523,7 +523,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>20</v>
@@ -532,7 +532,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>14</v>
@@ -571,19 +571,19 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>26</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>27</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -609,19 +609,19 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>29</v>
+      <c r="C4" s="13" t="s">
+        <v>24</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>26</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>27</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>

</xml_diff>